<commit_message>
feat: source file name
</commit_message>
<xml_diff>
--- a/combined_data.xlsx
+++ b/combined_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,684 +436,713 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Source File</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Eldon Base for stackable storage shelf, platinum</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Muhammed MacIntyre</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>-213.25</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>38.94</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SampleCSVFile_2kb_2.csv</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>1.7 Cubic Foot Compact "Cube" Office Refrigerators</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Barry French</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>293</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>457.81</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>208.16</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>68.02</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>Appliances</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>0.58</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>R380</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Clay Rozendal</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>483</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>1198.97</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>195.99</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>3.99</v>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>Telephones and Communication</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>0.58</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="n">
         <v>5</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Holmes HEPA Air Purifier</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Carlos Soltero</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>515</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>30.94</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>21.78</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>5.94</v>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>Appliances</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="n">
         <v>6</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>G.E. Longer-Life Indoor Recessed Floodlight Bulbs</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Carlos Soltero</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>515</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>4.43</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>6.64</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>4.95</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>Office Furnishings</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>0.37</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="n">
         <v>7</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Angle-D Binders with Locking Rings, Label Holders</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Carl Jackson</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>613</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>-54.04</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>7.3</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>7.72</v>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I6" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>Binders and Binder Accessories</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>0.38</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="n">
         <v>8</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>SAFCO Mobile Desk Side File, Wire Frame</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Carl Jackson</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>613</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>127.7</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>42.76</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>6.22</v>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="n">
         <v>9</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>SAFCO Commercial Wire Shelving, Black</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Monica Federle</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>643</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>-695.26</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>138.14</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>35</v>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I8" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
         <v>10</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Xerox 198</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Dorothy Badders</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>678</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>-226.36</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>4.98</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>8.33</v>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I9" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
           <t>Paper</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>0.38</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SampleCSVFile_2kb.csv</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>2</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>1.7 Cubic Foot Compact "Cube" Office Refrigerators</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Barry French</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>293</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>457.81</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>208.16</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>68.02</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
           <t>Appliances</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>0.58</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="n">
         <v>4</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>R380</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Clay Rozendal</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>483</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>1198.97</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>195.99</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>3.99</v>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
           <t>Telephones and Communication</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.58</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="n">
         <v>5</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Holmes HEPA Air Purifier</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Carlos Soltero</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>515</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>30.94</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>21.78</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>5.94</v>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I12" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
           <t>Appliances</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="n">
         <v>6</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>G.E. Longer-Life Indoor Recessed Floodlight Bulbs</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Carlos Soltero</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>515</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>4.43</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>6.64</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>4.95</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I13" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
           <t>Office Furnishings</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>0.37</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="n">
         <v>7</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Angle-D Binders with Locking Rings, Label Holders</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Carl Jackson</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>613</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>-54.04</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>7.3</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>7.72</v>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I14" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
           <t>Binders and Binder Accessories</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>0.38</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="n">
         <v>8</v>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>SAFCO Mobile Desk Side File, Wire Frame</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Carl Jackson</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>613</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>127.7</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>42.76</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>6.22</v>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
         <v>9</v>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>SAFCO Commercial Wire Shelving, Black</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Monica Federle</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>643</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>-695.26</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>138.14</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>35</v>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I16" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
           <t>Storage &amp; Organization</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="n">
         <v>10</v>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Xerox 198</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Dorothy Badders</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>678</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>-226.36</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>4.98</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>8.33</v>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Nunavut</t>
-        </is>
-      </c>
       <c r="I17" t="inlineStr">
         <is>
+          <t>Nunavut</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
           <t>Paper</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.38</v>
       </c>
     </row>

</xml_diff>